<commit_message>
Fix SE and T calculation
Recalculate SE and T, Changed description of hypothesis, S of two sample
croup.
</commit_message>
<xml_diff>
--- a/Origin data/stroopdata.xlsx
+++ b/Origin data/stroopdata.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="stroopdata" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -746,6 +746,930 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-TW"/>
+              <a:t>Standard deviation</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-TW" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="zh-TW"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>stroopdata!$A$1:$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Congruent</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Incongruent</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>stroopdata!$A$34:$B$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3.5593579576451955</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.7970571224691376</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="388836416"/>
+        <c:axId val="388836024"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="388836416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="388836024"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="388836024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="388836416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-TW"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="圖表 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
@@ -1011,16 +1935,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.375" customWidth="1"/>
     <col min="2" max="2" width="10.875" customWidth="1"/>
     <col min="3" max="3" width="22.875" customWidth="1"/>
-    <col min="4" max="4" width="14.75" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="14.875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="14.75" customWidth="1"/>
+    <col min="5" max="5" width="14.875" customWidth="1"/>
     <col min="6" max="6" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1056,11 +1981,12 @@
         <v>7.1989999999999981</v>
       </c>
       <c r="D2">
-        <f>(A2-A32)^2</f>
+        <f>(A2-$A$32)^2</f>
         <v>3.8892770156250007</v>
       </c>
       <c r="E2">
-        <v>7.4961876739999997</v>
+        <f>(B2-$B$32)^2</f>
+        <v>7.4961876736111321</v>
       </c>
       <c r="F2">
         <f>(C2-$C$32)^2</f>
@@ -1079,13 +2005,15 @@
         <v>1.9499999999999993</v>
       </c>
       <c r="D3">
-        <v>7.5069150159999998</v>
+        <f t="shared" ref="D3:D25" si="1">(A3-$A$32)^2</f>
+        <v>7.5069150156249975</v>
       </c>
       <c r="E3">
-        <v>10.725079170000001</v>
+        <f t="shared" ref="E3:E25" si="2">(B3-$B$32)^2</f>
+        <v>10.72507917361113</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F25" si="1">(C3-$C$32)^2</f>
+        <f t="shared" ref="F3:F25" si="3">(C3-$C$32)^2</f>
         <v>36.177718793402754</v>
       </c>
     </row>
@@ -1101,13 +2029,15 @@
         <v>11.649999999999999</v>
       </c>
       <c r="D4">
-        <v>20.13429077</v>
+        <f t="shared" si="1"/>
+        <v>20.134290765625007</v>
       </c>
       <c r="E4">
-        <v>0.64307033999999996</v>
+        <f t="shared" si="2"/>
+        <v>0.64307034027778409</v>
       </c>
       <c r="F4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>13.580760460069452</v>
       </c>
     </row>
@@ -1123,13 +2053,15 @@
         <v>7.0569999999999986</v>
       </c>
       <c r="D5">
-        <v>29.388596270000001</v>
+        <f t="shared" si="1"/>
+        <v>29.388596265625001</v>
       </c>
       <c r="E5">
-        <v>40.055186169999999</v>
+        <f t="shared" si="2"/>
+        <v>40.055186173611155</v>
       </c>
       <c r="F5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.8240857100694422</v>
       </c>
     </row>
@@ -1145,13 +2077,15 @@
         <v>8.1340000000000003</v>
       </c>
       <c r="D6">
-        <v>0.38176951599999998</v>
+        <f t="shared" si="1"/>
+        <v>0.38176951562499967</v>
       </c>
       <c r="E6">
-        <v>0.61950017400000001</v>
+        <f t="shared" si="2"/>
+        <v>0.61950017361110832</v>
       </c>
       <c r="F6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.8631460069445447E-2</v>
       </c>
     </row>
@@ -1167,13 +2101,15 @@
         <v>8.64</v>
       </c>
       <c r="D7">
-        <v>3.2874222660000001</v>
+        <f t="shared" si="1"/>
+        <v>3.2874222656250045</v>
       </c>
       <c r="E7">
-        <v>1.2948543400000001</v>
+        <f t="shared" si="2"/>
+        <v>1.2948543402777835</v>
       </c>
       <c r="F7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.4559062934027821</v>
       </c>
     </row>
@@ -1189,13 +2125,15 @@
         <v>9.879999999999999</v>
       </c>
       <c r="D8">
-        <v>0.41072076600000001</v>
+        <f t="shared" si="1"/>
+        <v>0.41072076562499926</v>
       </c>
       <c r="E8">
-        <v>6.5335620069999996</v>
+        <f t="shared" si="2"/>
+        <v>6.5335620069444271</v>
       </c>
       <c r="F8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.6680229600694507</v>
       </c>
     </row>
@@ -1211,13 +2149,15 @@
         <v>8.4069999999999983</v>
       </c>
       <c r="D9">
-        <v>25.64536202</v>
+        <f t="shared" si="1"/>
+        <v>25.645362015625008</v>
       </c>
       <c r="E9">
-        <v>21.362113669999999</v>
+        <f t="shared" si="2"/>
+        <v>21.362113673611152</v>
       </c>
       <c r="F9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.1955482100694452</v>
       </c>
     </row>
@@ -1233,13 +2173,15 @@
         <v>11.361000000000001</v>
       </c>
       <c r="D10">
-        <v>21.62366252</v>
+        <f t="shared" si="1"/>
+        <v>21.623662515625011</v>
       </c>
       <c r="E10">
-        <v>1.572307007</v>
+        <f t="shared" si="2"/>
+        <v>1.5723070069444498</v>
       </c>
       <c r="F10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>11.5342310434028</v>
       </c>
     </row>
@@ -1255,13 +2197,15 @@
         <v>11.802</v>
       </c>
       <c r="D11">
-        <v>0.183933766</v>
+        <f t="shared" si="1"/>
+        <v>0.18393376562499972</v>
       </c>
       <c r="E11">
-        <v>18.199467009999999</v>
+        <f t="shared" si="2"/>
+        <v>18.199467006944424</v>
       </c>
       <c r="F11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>14.724167793402795</v>
       </c>
     </row>
@@ -1277,13 +2221,15 @@
         <v>2.1960000000000015</v>
       </c>
       <c r="D12">
-        <v>68.506659769999999</v>
+        <f t="shared" si="1"/>
+        <v>68.506659765624974</v>
       </c>
       <c r="E12">
-        <v>6.2904820069999996</v>
+        <f t="shared" si="2"/>
+        <v>6.290482006944436</v>
       </c>
       <c r="F12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>33.278957293402733</v>
       </c>
     </row>
@@ -1299,13 +2245,15 @@
         <v>3.3459999999999983</v>
       </c>
       <c r="D13">
-        <v>1.554697266</v>
+        <f t="shared" si="1"/>
+        <v>1.5546972656249982</v>
       </c>
       <c r="E13">
-        <v>11.36982201</v>
+        <f t="shared" si="2"/>
+        <v>11.369822006944473</v>
       </c>
       <c r="F13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>21.333236460069436</v>
       </c>
     </row>
@@ -1321,13 +2269,15 @@
         <v>2.4370000000000012</v>
       </c>
       <c r="D14">
-        <v>1.044228516</v>
+        <f t="shared" si="1"/>
+        <v>1.0442285156249993</v>
       </c>
       <c r="E14">
-        <v>20.30328501</v>
+        <f t="shared" si="2"/>
+        <v>20.303285006944453</v>
       </c>
       <c r="F14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>30.556480710069401</v>
       </c>
     </row>
@@ -1343,13 +2293,15 @@
         <v>3.4009999999999998</v>
       </c>
       <c r="D15">
-        <v>8.2821645159999999</v>
+        <f t="shared" si="1"/>
+        <v>8.2821645156249861</v>
       </c>
       <c r="E15">
-        <v>2.8423150069999998</v>
+        <f t="shared" si="2"/>
+        <v>2.8423150069444589</v>
       </c>
       <c r="F15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>20.828194376736089</v>
       </c>
     </row>
@@ -1365,13 +2317,15 @@
         <v>17.055000000000003</v>
       </c>
       <c r="D16">
-        <v>17.213163770000001</v>
+        <f t="shared" si="1"/>
+        <v>17.213163765624987</v>
       </c>
       <c r="E16">
-        <v>175.27332749999999</v>
+        <f t="shared" si="2"/>
+        <v>175.27332750694444</v>
       </c>
       <c r="F16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>82.631887543402897</v>
       </c>
     </row>
@@ -1387,13 +2341,15 @@
         <v>10.028</v>
       </c>
       <c r="D17">
-        <v>3.6907212660000002</v>
+        <f t="shared" si="1"/>
+        <v>3.6907212656249997</v>
       </c>
       <c r="E17">
-        <v>2.0187673999999999E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.0187673611110735E-2</v>
       </c>
       <c r="F17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.2568286267361239</v>
       </c>
     </row>
@@ -1409,13 +2365,15 @@
         <v>6.6439999999999984</v>
       </c>
       <c r="D18">
-        <v>19.74802502</v>
+        <f t="shared" si="1"/>
+        <v>19.748025015625004</v>
       </c>
       <c r="E18">
-        <v>9.7536495070000004</v>
+        <f t="shared" si="2"/>
+        <v>9.7536495069444236</v>
       </c>
       <c r="F18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.7444906267361087</v>
       </c>
     </row>
@@ -1431,13 +2389,15 @@
         <v>9.7899999999999991</v>
       </c>
       <c r="D19">
-        <v>11.64259702</v>
+        <f t="shared" si="1"/>
+        <v>11.642597015625009</v>
       </c>
       <c r="E19">
-        <v>2.5183045069999999</v>
+        <f t="shared" si="2"/>
+        <v>2.5183045069444576</v>
       </c>
       <c r="F19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.331385460069451</v>
       </c>
     </row>
@@ -1453,13 +2413,15 @@
         <v>6.0810000000000013</v>
       </c>
       <c r="D20">
-        <v>7.3285257660000003</v>
+        <f t="shared" si="1"/>
+        <v>7.3285257656250069</v>
       </c>
       <c r="E20">
-        <v>21.076515839999999</v>
+        <f t="shared" si="2"/>
+        <v>21.076515840277796</v>
       </c>
       <c r="F20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.5486710434027628</v>
       </c>
     </row>
@@ -1475,13 +2437,15 @@
         <v>21.918999999999997</v>
       </c>
       <c r="D21">
-        <v>2.8295445159999999</v>
+        <f t="shared" si="1"/>
+        <v>2.8295445156250034</v>
       </c>
       <c r="E21">
-        <v>150.60402930000001</v>
+        <f t="shared" si="2"/>
+        <v>150.60402934027763</v>
       </c>
       <c r="F21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>194.71993021006946</v>
       </c>
     </row>
@@ -1497,13 +2461,15 @@
         <v>10.949999999999998</v>
       </c>
       <c r="D22">
-        <v>1.225725766</v>
+        <f t="shared" si="1"/>
+        <v>1.2257257656249998</v>
       </c>
       <c r="E22">
-        <v>3.5271970069999998</v>
+        <f t="shared" si="2"/>
+        <v>3.5271970069444287</v>
       </c>
       <c r="F22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8.9114687934027792</v>
       </c>
     </row>
@@ -1519,13 +2485,15 @@
         <v>3.7270000000000003</v>
       </c>
       <c r="D23">
-        <v>3.3078516000000002E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.3078515624999923E-2</v>
       </c>
       <c r="E23">
-        <v>16.45046001</v>
+        <f t="shared" si="2"/>
+        <v>16.450460006944457</v>
       </c>
       <c r="F23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>17.958878210069418</v>
       </c>
       <c r="I23">
@@ -1562,13 +2530,15 @@
         <v>2.347999999999999</v>
       </c>
       <c r="D24">
-        <v>32.022866270000002</v>
+        <f t="shared" si="1"/>
+        <v>32.022866265624998</v>
       </c>
       <c r="E24">
-        <v>1.771007E-3</v>
+        <f t="shared" si="2"/>
+        <v>1.7710069444442133E-3</v>
       </c>
       <c r="F24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>31.548348626736093</v>
       </c>
       <c r="I24">
@@ -1605,13 +2575,15 @@
         <v>5.1529999999999987</v>
       </c>
       <c r="D25">
-        <v>3.8137207659999999</v>
+        <f t="shared" si="1"/>
+        <v>3.8137207656250021</v>
       </c>
       <c r="E25">
-        <v>0.73773783999999998</v>
+        <f t="shared" si="2"/>
+        <v>0.73773784027778211</v>
       </c>
       <c r="F25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.9061723767361034</v>
       </c>
       <c r="I25">
@@ -1763,14 +2735,16 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30">
+        <f>A28-1</f>
         <v>23</v>
       </c>
       <c r="B30">
+        <f>B28-1</f>
         <v>23</v>
       </c>
       <c r="E30">
         <f>C34/C36</f>
-        <v>4.7958315233127191</v>
+        <v>4.8989794855663558</v>
       </c>
       <c r="I30">
         <v>12.13</v>
@@ -1828,10 +2802,12 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32">
+        <f>AVERAGE(A2:A25)</f>
         <v>14.051125000000001</v>
       </c>
       <c r="B32">
-        <v>22.015916669999999</v>
+        <f>AVERAGE(B2:B25)</f>
+        <v>22.015916666666669</v>
       </c>
       <c r="C32">
         <f>AVERAGE(C2:C25)</f>
@@ -1893,10 +2869,12 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>3.4844157130000002</v>
+        <f>SQRT(SUM(D2:D25)/A30)</f>
+        <v>3.5593579576451955</v>
       </c>
       <c r="B34">
-        <v>4.6960551349999999</v>
+        <f>SQRT(SUM(E2:E25)/B30)</f>
+        <v>4.7970571224691376</v>
       </c>
       <c r="C34">
         <f>SQRT(SUM(F2:F25)/B30)</f>
@@ -1958,8 +2936,8 @@
         <v>1.1695142009999999</v>
       </c>
       <c r="C36">
-        <f>C34/SQRT(B30)</f>
-        <v>1.0143865327026076</v>
+        <f>C34/SQRT(B28)</f>
+        <v>0.99302863477834025</v>
       </c>
       <c r="I36">
         <v>14.669</v>
@@ -2030,6 +3008,10 @@
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f>SQRT(SUM(D2:D25)/A30)</f>
+        <v>3.5593579576451955</v>
+      </c>
       <c r="I39">
         <v>15.298</v>
       </c>
@@ -2399,5 +3381,6 @@
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="119" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>